<commit_message>
Add proper clean_df for test and train
</commit_message>
<xml_diff>
--- a/dataset_test.xlsx
+++ b/dataset_test.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pclement/dslr/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="19420" tabRatio="500"/>
+    <workbookView xWindow="1460" yWindow="460" windowWidth="49740" windowHeight="22740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="dataset_test" localSheetId="0">Feuil1!$A$1:$S$401</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -17601,6 +17606,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -17932,9 +17942,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A302" workbookViewId="0">
+      <selection activeCell="H322" sqref="H322"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
@@ -17955,7 +17967,7 @@
     <col min="19" max="19" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -18014,7 +18026,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -18070,7 +18082,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -18126,7 +18138,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -18182,7 +18194,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -18229,7 +18241,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -18282,7 +18294,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -18338,7 +18350,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -18394,7 +18406,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -18450,7 +18462,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -18506,7 +18518,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -18562,7 +18574,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -18618,7 +18630,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -18671,7 +18683,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -18727,7 +18739,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -18783,7 +18795,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -18839,7 +18851,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -18892,7 +18904,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -18948,7 +18960,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -19004,7 +19016,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -19060,7 +19072,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -19116,7 +19128,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -19169,7 +19181,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -19225,7 +19237,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -19281,7 +19293,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -19337,7 +19349,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -19390,7 +19402,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -19446,7 +19458,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -19502,7 +19514,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -19555,7 +19567,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -19611,7 +19623,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -19667,7 +19679,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -19723,7 +19735,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -19776,7 +19788,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -19832,7 +19844,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -19888,7 +19900,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -19944,7 +19956,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -20000,7 +20012,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -20056,7 +20068,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -20112,7 +20124,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -20168,7 +20180,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -20224,7 +20236,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -20280,7 +20292,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -20336,7 +20348,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -20386,7 +20398,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="45" spans="1:19">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -20439,7 +20451,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="46" spans="1:19">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -20492,7 +20504,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -20548,7 +20560,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="48" spans="1:19">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -20604,7 +20616,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -20660,7 +20672,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -20716,7 +20728,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -20772,7 +20784,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
@@ -20828,7 +20840,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="53" spans="1:19">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -20884,7 +20896,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
@@ -20940,7 +20952,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -20996,7 +21008,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
@@ -21052,7 +21064,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
@@ -21108,7 +21120,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="58" spans="1:19">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
@@ -21161,7 +21173,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -21217,7 +21229,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="60" spans="1:19">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
@@ -21273,7 +21285,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="61" spans="1:19">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
@@ -21329,7 +21341,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="62" spans="1:19">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
@@ -21385,7 +21397,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="63" spans="1:19">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
@@ -21441,7 +21453,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="64" spans="1:19">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
@@ -21497,7 +21509,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="65" spans="1:19">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
@@ -21553,7 +21565,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="66" spans="1:19">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
@@ -21609,7 +21621,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="67" spans="1:19">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
@@ -21665,7 +21677,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="68" spans="1:19">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
@@ -21718,7 +21730,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="69" spans="1:19">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
@@ -21774,7 +21786,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="70" spans="1:19">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
@@ -21827,7 +21839,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="71" spans="1:19">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
@@ -21883,7 +21895,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="72" spans="1:19">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
@@ -21939,7 +21951,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="73" spans="1:19">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
@@ -21995,7 +22007,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="74" spans="1:19">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>72</v>
       </c>
@@ -22045,7 +22057,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="75" spans="1:19">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>73</v>
       </c>
@@ -22101,7 +22113,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="76" spans="1:19">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>74</v>
       </c>
@@ -22154,7 +22166,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="77" spans="1:19">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>75</v>
       </c>
@@ -22207,7 +22219,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="78" spans="1:19">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>76</v>
       </c>
@@ -22263,7 +22275,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="79" spans="1:19">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>77</v>
       </c>
@@ -22316,7 +22328,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="80" spans="1:19">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>78</v>
       </c>
@@ -22369,7 +22381,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="81" spans="1:19">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>79</v>
       </c>
@@ -22422,7 +22434,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="82" spans="1:19">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>80</v>
       </c>
@@ -22478,7 +22490,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="83" spans="1:19">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>81</v>
       </c>
@@ -22534,7 +22546,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="84" spans="1:19">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>82</v>
       </c>
@@ -22590,7 +22602,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="85" spans="1:19">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>83</v>
       </c>
@@ -22646,7 +22658,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="86" spans="1:19">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>84</v>
       </c>
@@ -22699,7 +22711,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="87" spans="1:19">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>85</v>
       </c>
@@ -22755,7 +22767,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="88" spans="1:19">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>86</v>
       </c>
@@ -22811,7 +22823,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="89" spans="1:19">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>87</v>
       </c>
@@ -22867,7 +22879,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="90" spans="1:19">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>88</v>
       </c>
@@ -22923,7 +22935,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="91" spans="1:19">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>89</v>
       </c>
@@ -22979,7 +22991,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="92" spans="1:19">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>90</v>
       </c>
@@ -23032,7 +23044,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="93" spans="1:19">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>91</v>
       </c>
@@ -23088,7 +23100,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="94" spans="1:19">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>92</v>
       </c>
@@ -23144,7 +23156,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="95" spans="1:19">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>93</v>
       </c>
@@ -23197,7 +23209,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="96" spans="1:19">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>94</v>
       </c>
@@ -23253,7 +23265,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="97" spans="1:19">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>95</v>
       </c>
@@ -23309,7 +23321,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="98" spans="1:19">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>96</v>
       </c>
@@ -23365,7 +23377,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="99" spans="1:19">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>97</v>
       </c>
@@ -23421,7 +23433,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="100" spans="1:19">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>98</v>
       </c>
@@ -23471,7 +23483,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="101" spans="1:19">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>99</v>
       </c>
@@ -23527,7 +23539,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="102" spans="1:19">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>100</v>
       </c>
@@ -23583,7 +23595,7 @@
         <v>1502</v>
       </c>
     </row>
-    <row r="103" spans="1:19">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>101</v>
       </c>
@@ -23639,7 +23651,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="104" spans="1:19">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>102</v>
       </c>
@@ -23695,7 +23707,7 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="105" spans="1:19">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>103</v>
       </c>
@@ -23748,7 +23760,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="106" spans="1:19">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>104</v>
       </c>
@@ -23804,7 +23816,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="107" spans="1:19">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>105</v>
       </c>
@@ -23854,7 +23866,7 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="108" spans="1:19">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>106</v>
       </c>
@@ -23910,7 +23922,7 @@
         <v>1587</v>
       </c>
     </row>
-    <row r="109" spans="1:19">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>107</v>
       </c>
@@ -23963,7 +23975,7 @@
         <v>1601</v>
       </c>
     </row>
-    <row r="110" spans="1:19">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>108</v>
       </c>
@@ -24013,7 +24025,7 @@
         <v>1614</v>
       </c>
     </row>
-    <row r="111" spans="1:19">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>109</v>
       </c>
@@ -24066,7 +24078,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="112" spans="1:19">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>110</v>
       </c>
@@ -24122,7 +24134,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="113" spans="1:19">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>111</v>
       </c>
@@ -24178,7 +24190,7 @@
         <v>1658</v>
       </c>
     </row>
-    <row r="114" spans="1:19">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>112</v>
       </c>
@@ -24234,7 +24246,7 @@
         <v>1673</v>
       </c>
     </row>
-    <row r="115" spans="1:19">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>113</v>
       </c>
@@ -24290,7 +24302,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="116" spans="1:19">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>114</v>
       </c>
@@ -24343,7 +24355,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="117" spans="1:19">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>115</v>
       </c>
@@ -24399,7 +24411,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="118" spans="1:19">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>116</v>
       </c>
@@ -24452,7 +24464,7 @@
         <v>1729</v>
       </c>
     </row>
-    <row r="119" spans="1:19">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>117</v>
       </c>
@@ -24505,7 +24517,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="120" spans="1:19">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>118</v>
       </c>
@@ -24558,7 +24570,7 @@
         <v>1757</v>
       </c>
     </row>
-    <row r="121" spans="1:19">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>119</v>
       </c>
@@ -24614,7 +24626,7 @@
         <v>1772</v>
       </c>
     </row>
-    <row r="122" spans="1:19">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>120</v>
       </c>
@@ -24670,7 +24682,7 @@
         <v>1786</v>
       </c>
     </row>
-    <row r="123" spans="1:19">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>121</v>
       </c>
@@ -24726,7 +24738,7 @@
         <v>1801</v>
       </c>
     </row>
-    <row r="124" spans="1:19">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>122</v>
       </c>
@@ -24782,7 +24794,7 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="125" spans="1:19">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>123</v>
       </c>
@@ -24838,7 +24850,7 @@
         <v>1830</v>
       </c>
     </row>
-    <row r="126" spans="1:19">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>124</v>
       </c>
@@ -24894,7 +24906,7 @@
         <v>1845</v>
       </c>
     </row>
-    <row r="127" spans="1:19">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>125</v>
       </c>
@@ -24950,7 +24962,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="128" spans="1:19">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>126</v>
       </c>
@@ -25006,7 +25018,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="129" spans="1:19">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>127</v>
       </c>
@@ -25062,7 +25074,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="130" spans="1:19">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>128</v>
       </c>
@@ -25118,7 +25130,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="131" spans="1:19">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>129</v>
       </c>
@@ -25174,7 +25186,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="132" spans="1:19">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>130</v>
       </c>
@@ -25230,7 +25242,7 @@
         <v>1935</v>
       </c>
     </row>
-    <row r="133" spans="1:19">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>131</v>
       </c>
@@ -25286,7 +25298,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="134" spans="1:19">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>132</v>
       </c>
@@ -25342,7 +25354,7 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="135" spans="1:19">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>133</v>
       </c>
@@ -25398,7 +25410,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="136" spans="1:19">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>134</v>
       </c>
@@ -25454,7 +25466,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="137" spans="1:19">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>135</v>
       </c>
@@ -25507,7 +25519,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="138" spans="1:19">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>136</v>
       </c>
@@ -25563,7 +25575,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="139" spans="1:19">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>137</v>
       </c>
@@ -25619,7 +25631,7 @@
         <v>2039</v>
       </c>
     </row>
-    <row r="140" spans="1:19">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>138</v>
       </c>
@@ -25675,7 +25687,7 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="141" spans="1:19">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>139</v>
       </c>
@@ -25731,7 +25743,7 @@
         <v>2069</v>
       </c>
     </row>
-    <row r="142" spans="1:19">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>140</v>
       </c>
@@ -25787,7 +25799,7 @@
         <v>2083</v>
       </c>
     </row>
-    <row r="143" spans="1:19">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>141</v>
       </c>
@@ -25843,7 +25855,7 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="144" spans="1:19">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>142</v>
       </c>
@@ -25896,7 +25908,7 @@
         <v>2112</v>
       </c>
     </row>
-    <row r="145" spans="1:19">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>143</v>
       </c>
@@ -25952,7 +25964,7 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="146" spans="1:19">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>144</v>
       </c>
@@ -26008,7 +26020,7 @@
         <v>2142</v>
       </c>
     </row>
-    <row r="147" spans="1:19">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>145</v>
       </c>
@@ -26064,7 +26076,7 @@
         <v>2157</v>
       </c>
     </row>
-    <row r="148" spans="1:19">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>146</v>
       </c>
@@ -26117,7 +26129,7 @@
         <v>2171</v>
       </c>
     </row>
-    <row r="149" spans="1:19">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>147</v>
       </c>
@@ -26173,7 +26185,7 @@
         <v>2186</v>
       </c>
     </row>
-    <row r="150" spans="1:19">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>148</v>
       </c>
@@ -26229,7 +26241,7 @@
         <v>2201</v>
       </c>
     </row>
-    <row r="151" spans="1:19">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>149</v>
       </c>
@@ -26282,7 +26294,7 @@
         <v>2214</v>
       </c>
     </row>
-    <row r="152" spans="1:19">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>150</v>
       </c>
@@ -26338,7 +26350,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="153" spans="1:19">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>151</v>
       </c>
@@ -26394,7 +26406,7 @@
         <v>2244</v>
       </c>
     </row>
-    <row r="154" spans="1:19">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>152</v>
       </c>
@@ -26450,7 +26462,7 @@
         <v>2258</v>
       </c>
     </row>
-    <row r="155" spans="1:19">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>153</v>
       </c>
@@ -26506,7 +26518,7 @@
         <v>2273</v>
       </c>
     </row>
-    <row r="156" spans="1:19">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>154</v>
       </c>
@@ -26562,7 +26574,7 @@
         <v>2288</v>
       </c>
     </row>
-    <row r="157" spans="1:19">
+    <row r="157" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>155</v>
       </c>
@@ -26618,7 +26630,7 @@
         <v>2303</v>
       </c>
     </row>
-    <row r="158" spans="1:19">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>156</v>
       </c>
@@ -26674,7 +26686,7 @@
         <v>2318</v>
       </c>
     </row>
-    <row r="159" spans="1:19">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>157</v>
       </c>
@@ -26730,7 +26742,7 @@
         <v>2333</v>
       </c>
     </row>
-    <row r="160" spans="1:19">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>158</v>
       </c>
@@ -26783,7 +26795,7 @@
         <v>2347</v>
       </c>
     </row>
-    <row r="161" spans="1:19">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>159</v>
       </c>
@@ -26836,7 +26848,7 @@
         <v>2361</v>
       </c>
     </row>
-    <row r="162" spans="1:19">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>160</v>
       </c>
@@ -26892,7 +26904,7 @@
         <v>2376</v>
       </c>
     </row>
-    <row r="163" spans="1:19">
+    <row r="163" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>161</v>
       </c>
@@ -26948,7 +26960,7 @@
         <v>2391</v>
       </c>
     </row>
-    <row r="164" spans="1:19">
+    <row r="164" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>162</v>
       </c>
@@ -27004,7 +27016,7 @@
         <v>2406</v>
       </c>
     </row>
-    <row r="165" spans="1:19">
+    <row r="165" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>163</v>
       </c>
@@ -27060,7 +27072,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="166" spans="1:19">
+    <row r="166" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>164</v>
       </c>
@@ -27116,7 +27128,7 @@
         <v>2436</v>
       </c>
     </row>
-    <row r="167" spans="1:19">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>165</v>
       </c>
@@ -27172,7 +27184,7 @@
         <v>2451</v>
       </c>
     </row>
-    <row r="168" spans="1:19">
+    <row r="168" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>166</v>
       </c>
@@ -27228,7 +27240,7 @@
         <v>2466</v>
       </c>
     </row>
-    <row r="169" spans="1:19">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>167</v>
       </c>
@@ -27281,7 +27293,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="170" spans="1:19">
+    <row r="170" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>168</v>
       </c>
@@ -27337,7 +27349,7 @@
         <v>2494</v>
       </c>
     </row>
-    <row r="171" spans="1:19">
+    <row r="171" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>169</v>
       </c>
@@ -27393,7 +27405,7 @@
         <v>2509</v>
       </c>
     </row>
-    <row r="172" spans="1:19">
+    <row r="172" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>170</v>
       </c>
@@ -27449,7 +27461,7 @@
         <v>2522</v>
       </c>
     </row>
-    <row r="173" spans="1:19">
+    <row r="173" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>171</v>
       </c>
@@ -27505,7 +27517,7 @@
         <v>2537</v>
       </c>
     </row>
-    <row r="174" spans="1:19">
+    <row r="174" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>172</v>
       </c>
@@ -27561,7 +27573,7 @@
         <v>2552</v>
       </c>
     </row>
-    <row r="175" spans="1:19">
+    <row r="175" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>173</v>
       </c>
@@ -27614,7 +27626,7 @@
         <v>2566</v>
       </c>
     </row>
-    <row r="176" spans="1:19">
+    <row r="176" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>174</v>
       </c>
@@ -27667,7 +27679,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="177" spans="1:19">
+    <row r="177" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>175</v>
       </c>
@@ -27723,7 +27735,7 @@
         <v>2595</v>
       </c>
     </row>
-    <row r="178" spans="1:19">
+    <row r="178" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>176</v>
       </c>
@@ -27773,7 +27785,7 @@
         <v>2607</v>
       </c>
     </row>
-    <row r="179" spans="1:19">
+    <row r="179" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>177</v>
       </c>
@@ -27829,7 +27841,7 @@
         <v>2622</v>
       </c>
     </row>
-    <row r="180" spans="1:19">
+    <row r="180" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>178</v>
       </c>
@@ -27885,7 +27897,7 @@
         <v>2637</v>
       </c>
     </row>
-    <row r="181" spans="1:19">
+    <row r="181" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>179</v>
       </c>
@@ -27941,7 +27953,7 @@
         <v>2652</v>
       </c>
     </row>
-    <row r="182" spans="1:19">
+    <row r="182" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>180</v>
       </c>
@@ -27997,7 +28009,7 @@
         <v>2667</v>
       </c>
     </row>
-    <row r="183" spans="1:19">
+    <row r="183" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>181</v>
       </c>
@@ -28050,7 +28062,7 @@
         <v>2681</v>
       </c>
     </row>
-    <row r="184" spans="1:19">
+    <row r="184" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>182</v>
       </c>
@@ -28106,7 +28118,7 @@
         <v>2696</v>
       </c>
     </row>
-    <row r="185" spans="1:19">
+    <row r="185" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>183</v>
       </c>
@@ -28162,7 +28174,7 @@
         <v>2709</v>
       </c>
     </row>
-    <row r="186" spans="1:19">
+    <row r="186" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>184</v>
       </c>
@@ -28218,7 +28230,7 @@
         <v>2724</v>
       </c>
     </row>
-    <row r="187" spans="1:19">
+    <row r="187" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>185</v>
       </c>
@@ -28274,7 +28286,7 @@
         <v>2739</v>
       </c>
     </row>
-    <row r="188" spans="1:19">
+    <row r="188" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>186</v>
       </c>
@@ -28330,7 +28342,7 @@
         <v>2754</v>
       </c>
     </row>
-    <row r="189" spans="1:19">
+    <row r="189" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>187</v>
       </c>
@@ -28386,7 +28398,7 @@
         <v>2769</v>
       </c>
     </row>
-    <row r="190" spans="1:19">
+    <row r="190" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>188</v>
       </c>
@@ -28442,7 +28454,7 @@
         <v>2784</v>
       </c>
     </row>
-    <row r="191" spans="1:19">
+    <row r="191" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>189</v>
       </c>
@@ -28498,7 +28510,7 @@
         <v>2799</v>
       </c>
     </row>
-    <row r="192" spans="1:19">
+    <row r="192" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>190</v>
       </c>
@@ -28554,7 +28566,7 @@
         <v>2814</v>
       </c>
     </row>
-    <row r="193" spans="1:19">
+    <row r="193" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>191</v>
       </c>
@@ -28607,7 +28619,7 @@
         <v>2828</v>
       </c>
     </row>
-    <row r="194" spans="1:19">
+    <row r="194" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>192</v>
       </c>
@@ -28663,7 +28675,7 @@
         <v>2843</v>
       </c>
     </row>
-    <row r="195" spans="1:19">
+    <row r="195" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>193</v>
       </c>
@@ -28719,7 +28731,7 @@
         <v>2858</v>
       </c>
     </row>
-    <row r="196" spans="1:19">
+    <row r="196" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>194</v>
       </c>
@@ -28775,7 +28787,7 @@
         <v>2873</v>
       </c>
     </row>
-    <row r="197" spans="1:19">
+    <row r="197" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>195</v>
       </c>
@@ -28831,7 +28843,7 @@
         <v>2888</v>
       </c>
     </row>
-    <row r="198" spans="1:19">
+    <row r="198" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>196</v>
       </c>
@@ -28887,7 +28899,7 @@
         <v>2903</v>
       </c>
     </row>
-    <row r="199" spans="1:19">
+    <row r="199" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>197</v>
       </c>
@@ -28943,7 +28955,7 @@
         <v>2918</v>
       </c>
     </row>
-    <row r="200" spans="1:19">
+    <row r="200" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>198</v>
       </c>
@@ -28996,7 +29008,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="201" spans="1:19">
+    <row r="201" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>199</v>
       </c>
@@ -29052,7 +29064,7 @@
         <v>2947</v>
       </c>
     </row>
-    <row r="202" spans="1:19">
+    <row r="202" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>200</v>
       </c>
@@ -29108,7 +29120,7 @@
         <v>2962</v>
       </c>
     </row>
-    <row r="203" spans="1:19">
+    <row r="203" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>201</v>
       </c>
@@ -29164,7 +29176,7 @@
         <v>2977</v>
       </c>
     </row>
-    <row r="204" spans="1:19">
+    <row r="204" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>202</v>
       </c>
@@ -29220,7 +29232,7 @@
         <v>2992</v>
       </c>
     </row>
-    <row r="205" spans="1:19">
+    <row r="205" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>203</v>
       </c>
@@ -29276,7 +29288,7 @@
         <v>3007</v>
       </c>
     </row>
-    <row r="206" spans="1:19">
+    <row r="206" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>204</v>
       </c>
@@ -29332,7 +29344,7 @@
         <v>3022</v>
       </c>
     </row>
-    <row r="207" spans="1:19">
+    <row r="207" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>205</v>
       </c>
@@ -29388,7 +29400,7 @@
         <v>3037</v>
       </c>
     </row>
-    <row r="208" spans="1:19">
+    <row r="208" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>206</v>
       </c>
@@ -29444,7 +29456,7 @@
         <v>3052</v>
       </c>
     </row>
-    <row r="209" spans="1:19">
+    <row r="209" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>207</v>
       </c>
@@ -29500,7 +29512,7 @@
         <v>3067</v>
       </c>
     </row>
-    <row r="210" spans="1:19">
+    <row r="210" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>208</v>
       </c>
@@ -29556,7 +29568,7 @@
         <v>3082</v>
       </c>
     </row>
-    <row r="211" spans="1:19">
+    <row r="211" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>209</v>
       </c>
@@ -29609,7 +29621,7 @@
         <v>3096</v>
       </c>
     </row>
-    <row r="212" spans="1:19">
+    <row r="212" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>210</v>
       </c>
@@ -29665,7 +29677,7 @@
         <v>3111</v>
       </c>
     </row>
-    <row r="213" spans="1:19">
+    <row r="213" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>211</v>
       </c>
@@ -29721,7 +29733,7 @@
         <v>3126</v>
       </c>
     </row>
-    <row r="214" spans="1:19">
+    <row r="214" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>212</v>
       </c>
@@ -29777,7 +29789,7 @@
         <v>3141</v>
       </c>
     </row>
-    <row r="215" spans="1:19">
+    <row r="215" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>213</v>
       </c>
@@ -29833,7 +29845,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="216" spans="1:19">
+    <row r="216" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>214</v>
       </c>
@@ -29889,7 +29901,7 @@
         <v>3169</v>
       </c>
     </row>
-    <row r="217" spans="1:19">
+    <row r="217" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>215</v>
       </c>
@@ -29945,7 +29957,7 @@
         <v>3184</v>
       </c>
     </row>
-    <row r="218" spans="1:19">
+    <row r="218" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>216</v>
       </c>
@@ -30001,7 +30013,7 @@
         <v>3198</v>
       </c>
     </row>
-    <row r="219" spans="1:19">
+    <row r="219" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>217</v>
       </c>
@@ -30057,7 +30069,7 @@
         <v>3213</v>
       </c>
     </row>
-    <row r="220" spans="1:19">
+    <row r="220" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>218</v>
       </c>
@@ -30113,7 +30125,7 @@
         <v>3228</v>
       </c>
     </row>
-    <row r="221" spans="1:19">
+    <row r="221" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>219</v>
       </c>
@@ -30169,7 +30181,7 @@
         <v>3241</v>
       </c>
     </row>
-    <row r="222" spans="1:19">
+    <row r="222" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>220</v>
       </c>
@@ -30225,7 +30237,7 @@
         <v>3256</v>
       </c>
     </row>
-    <row r="223" spans="1:19">
+    <row r="223" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>221</v>
       </c>
@@ -30281,7 +30293,7 @@
         <v>3271</v>
       </c>
     </row>
-    <row r="224" spans="1:19">
+    <row r="224" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>222</v>
       </c>
@@ -30337,7 +30349,7 @@
         <v>3286</v>
       </c>
     </row>
-    <row r="225" spans="1:19">
+    <row r="225" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>223</v>
       </c>
@@ -30393,7 +30405,7 @@
         <v>3301</v>
       </c>
     </row>
-    <row r="226" spans="1:19">
+    <row r="226" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>224</v>
       </c>
@@ -30449,7 +30461,7 @@
         <v>3316</v>
       </c>
     </row>
-    <row r="227" spans="1:19">
+    <row r="227" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>225</v>
       </c>
@@ -30505,7 +30517,7 @@
         <v>3331</v>
       </c>
     </row>
-    <row r="228" spans="1:19">
+    <row r="228" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>226</v>
       </c>
@@ -30561,7 +30573,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="229" spans="1:19">
+    <row r="229" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>227</v>
       </c>
@@ -30617,7 +30629,7 @@
         <v>3359</v>
       </c>
     </row>
-    <row r="230" spans="1:19">
+    <row r="230" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>228</v>
       </c>
@@ -30673,7 +30685,7 @@
         <v>3374</v>
       </c>
     </row>
-    <row r="231" spans="1:19">
+    <row r="231" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>229</v>
       </c>
@@ -30729,7 +30741,7 @@
         <v>3388</v>
       </c>
     </row>
-    <row r="232" spans="1:19">
+    <row r="232" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>230</v>
       </c>
@@ -30785,7 +30797,7 @@
         <v>3403</v>
       </c>
     </row>
-    <row r="233" spans="1:19">
+    <row r="233" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>231</v>
       </c>
@@ -30838,7 +30850,7 @@
         <v>3417</v>
       </c>
     </row>
-    <row r="234" spans="1:19">
+    <row r="234" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>232</v>
       </c>
@@ -30894,7 +30906,7 @@
         <v>3431</v>
       </c>
     </row>
-    <row r="235" spans="1:19">
+    <row r="235" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>233</v>
       </c>
@@ -30950,7 +30962,7 @@
         <v>3446</v>
       </c>
     </row>
-    <row r="236" spans="1:19">
+    <row r="236" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>234</v>
       </c>
@@ -31006,7 +31018,7 @@
         <v>3460</v>
       </c>
     </row>
-    <row r="237" spans="1:19">
+    <row r="237" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>235</v>
       </c>
@@ -31062,7 +31074,7 @@
         <v>3474</v>
       </c>
     </row>
-    <row r="238" spans="1:19">
+    <row r="238" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>236</v>
       </c>
@@ -31118,7 +31130,7 @@
         <v>3489</v>
       </c>
     </row>
-    <row r="239" spans="1:19">
+    <row r="239" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>237</v>
       </c>
@@ -31174,7 +31186,7 @@
         <v>3504</v>
       </c>
     </row>
-    <row r="240" spans="1:19">
+    <row r="240" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>238</v>
       </c>
@@ -31230,7 +31242,7 @@
         <v>3519</v>
       </c>
     </row>
-    <row r="241" spans="1:19">
+    <row r="241" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>239</v>
       </c>
@@ -31280,7 +31292,7 @@
         <v>3532</v>
       </c>
     </row>
-    <row r="242" spans="1:19">
+    <row r="242" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>240</v>
       </c>
@@ -31336,7 +31348,7 @@
         <v>3546</v>
       </c>
     </row>
-    <row r="243" spans="1:19">
+    <row r="243" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>241</v>
       </c>
@@ -31392,7 +31404,7 @@
         <v>3561</v>
       </c>
     </row>
-    <row r="244" spans="1:19">
+    <row r="244" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>242</v>
       </c>
@@ -31448,7 +31460,7 @@
         <v>3576</v>
       </c>
     </row>
-    <row r="245" spans="1:19">
+    <row r="245" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>243</v>
       </c>
@@ -31504,7 +31516,7 @@
         <v>3589</v>
       </c>
     </row>
-    <row r="246" spans="1:19">
+    <row r="246" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>244</v>
       </c>
@@ -31560,7 +31572,7 @@
         <v>3604</v>
       </c>
     </row>
-    <row r="247" spans="1:19">
+    <row r="247" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>245</v>
       </c>
@@ -31616,7 +31628,7 @@
         <v>3619</v>
       </c>
     </row>
-    <row r="248" spans="1:19">
+    <row r="248" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>246</v>
       </c>
@@ -31672,7 +31684,7 @@
         <v>3634</v>
       </c>
     </row>
-    <row r="249" spans="1:19">
+    <row r="249" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>247</v>
       </c>
@@ -31728,7 +31740,7 @@
         <v>3649</v>
       </c>
     </row>
-    <row r="250" spans="1:19">
+    <row r="250" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>248</v>
       </c>
@@ -31778,7 +31790,7 @@
         <v>3662</v>
       </c>
     </row>
-    <row r="251" spans="1:19">
+    <row r="251" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>249</v>
       </c>
@@ -31834,7 +31846,7 @@
         <v>3677</v>
       </c>
     </row>
-    <row r="252" spans="1:19">
+    <row r="252" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>250</v>
       </c>
@@ -31887,7 +31899,7 @@
         <v>3691</v>
       </c>
     </row>
-    <row r="253" spans="1:19">
+    <row r="253" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>251</v>
       </c>
@@ -31943,7 +31955,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="254" spans="1:19">
+    <row r="254" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>252</v>
       </c>
@@ -31996,7 +32008,7 @@
         <v>3720</v>
       </c>
     </row>
-    <row r="255" spans="1:19">
+    <row r="255" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>253</v>
       </c>
@@ -32052,7 +32064,7 @@
         <v>3735</v>
       </c>
     </row>
-    <row r="256" spans="1:19">
+    <row r="256" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>254</v>
       </c>
@@ -32105,7 +32117,7 @@
         <v>3749</v>
       </c>
     </row>
-    <row r="257" spans="1:19">
+    <row r="257" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>255</v>
       </c>
@@ -32161,7 +32173,7 @@
         <v>3764</v>
       </c>
     </row>
-    <row r="258" spans="1:19">
+    <row r="258" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>256</v>
       </c>
@@ -32217,7 +32229,7 @@
         <v>3779</v>
       </c>
     </row>
-    <row r="259" spans="1:19">
+    <row r="259" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>257</v>
       </c>
@@ -32273,7 +32285,7 @@
         <v>3794</v>
       </c>
     </row>
-    <row r="260" spans="1:19">
+    <row r="260" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>258</v>
       </c>
@@ -32329,7 +32341,7 @@
         <v>3809</v>
       </c>
     </row>
-    <row r="261" spans="1:19">
+    <row r="261" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>259</v>
       </c>
@@ -32385,7 +32397,7 @@
         <v>3824</v>
       </c>
     </row>
-    <row r="262" spans="1:19">
+    <row r="262" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>260</v>
       </c>
@@ -32438,7 +32450,7 @@
         <v>3838</v>
       </c>
     </row>
-    <row r="263" spans="1:19">
+    <row r="263" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>261</v>
       </c>
@@ -32494,7 +32506,7 @@
         <v>3853</v>
       </c>
     </row>
-    <row r="264" spans="1:19">
+    <row r="264" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>262</v>
       </c>
@@ -32550,7 +32562,7 @@
         <v>3868</v>
       </c>
     </row>
-    <row r="265" spans="1:19">
+    <row r="265" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>263</v>
       </c>
@@ -32606,7 +32618,7 @@
         <v>3883</v>
       </c>
     </row>
-    <row r="266" spans="1:19">
+    <row r="266" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>264</v>
       </c>
@@ -32662,7 +32674,7 @@
         <v>3898</v>
       </c>
     </row>
-    <row r="267" spans="1:19">
+    <row r="267" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>265</v>
       </c>
@@ -32718,7 +32730,7 @@
         <v>3913</v>
       </c>
     </row>
-    <row r="268" spans="1:19">
+    <row r="268" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>266</v>
       </c>
@@ -32771,7 +32783,7 @@
         <v>3927</v>
       </c>
     </row>
-    <row r="269" spans="1:19">
+    <row r="269" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>267</v>
       </c>
@@ -32824,7 +32836,7 @@
         <v>2303</v>
       </c>
     </row>
-    <row r="270" spans="1:19">
+    <row r="270" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>268</v>
       </c>
@@ -32877,7 +32889,7 @@
         <v>3954</v>
       </c>
     </row>
-    <row r="271" spans="1:19">
+    <row r="271" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>269</v>
       </c>
@@ -32933,7 +32945,7 @@
         <v>3969</v>
       </c>
     </row>
-    <row r="272" spans="1:19">
+    <row r="272" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>270</v>
       </c>
@@ -32989,7 +33001,7 @@
         <v>3982</v>
       </c>
     </row>
-    <row r="273" spans="1:19">
+    <row r="273" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>271</v>
       </c>
@@ -33045,7 +33057,7 @@
         <v>3997</v>
       </c>
     </row>
-    <row r="274" spans="1:19">
+    <row r="274" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>272</v>
       </c>
@@ -33101,7 +33113,7 @@
         <v>4012</v>
       </c>
     </row>
-    <row r="275" spans="1:19">
+    <row r="275" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>273</v>
       </c>
@@ -33157,7 +33169,7 @@
         <v>4027</v>
       </c>
     </row>
-    <row r="276" spans="1:19">
+    <row r="276" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>274</v>
       </c>
@@ -33213,7 +33225,7 @@
         <v>4042</v>
       </c>
     </row>
-    <row r="277" spans="1:19">
+    <row r="277" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>275</v>
       </c>
@@ -33269,7 +33281,7 @@
         <v>4056</v>
       </c>
     </row>
-    <row r="278" spans="1:19">
+    <row r="278" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>276</v>
       </c>
@@ -33319,7 +33331,7 @@
         <v>4069</v>
       </c>
     </row>
-    <row r="279" spans="1:19">
+    <row r="279" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>277</v>
       </c>
@@ -33375,7 +33387,7 @@
         <v>4084</v>
       </c>
     </row>
-    <row r="280" spans="1:19">
+    <row r="280" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>278</v>
       </c>
@@ -33431,7 +33443,7 @@
         <v>4099</v>
       </c>
     </row>
-    <row r="281" spans="1:19">
+    <row r="281" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>279</v>
       </c>
@@ -33484,7 +33496,7 @@
         <v>4113</v>
       </c>
     </row>
-    <row r="282" spans="1:19">
+    <row r="282" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>280</v>
       </c>
@@ -33537,7 +33549,7 @@
         <v>4127</v>
       </c>
     </row>
-    <row r="283" spans="1:19">
+    <row r="283" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>281</v>
       </c>
@@ -33593,7 +33605,7 @@
         <v>4142</v>
       </c>
     </row>
-    <row r="284" spans="1:19">
+    <row r="284" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>282</v>
       </c>
@@ -33649,7 +33661,7 @@
         <v>4157</v>
       </c>
     </row>
-    <row r="285" spans="1:19">
+    <row r="285" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>283</v>
       </c>
@@ -33702,7 +33714,7 @@
         <v>4171</v>
       </c>
     </row>
-    <row r="286" spans="1:19">
+    <row r="286" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>284</v>
       </c>
@@ -33755,7 +33767,7 @@
         <v>4185</v>
       </c>
     </row>
-    <row r="287" spans="1:19">
+    <row r="287" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>285</v>
       </c>
@@ -33811,7 +33823,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="288" spans="1:19">
+    <row r="288" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>286</v>
       </c>
@@ -33864,7 +33876,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="289" spans="1:19">
+    <row r="289" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>287</v>
       </c>
@@ -33917,7 +33929,7 @@
         <v>4228</v>
       </c>
     </row>
-    <row r="290" spans="1:19">
+    <row r="290" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>288</v>
       </c>
@@ -33970,7 +33982,7 @@
         <v>4241</v>
       </c>
     </row>
-    <row r="291" spans="1:19">
+    <row r="291" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>289</v>
       </c>
@@ -34026,7 +34038,7 @@
         <v>4256</v>
       </c>
     </row>
-    <row r="292" spans="1:19">
+    <row r="292" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>290</v>
       </c>
@@ -34082,7 +34094,7 @@
         <v>4271</v>
       </c>
     </row>
-    <row r="293" spans="1:19">
+    <row r="293" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>291</v>
       </c>
@@ -34138,7 +34150,7 @@
         <v>4286</v>
       </c>
     </row>
-    <row r="294" spans="1:19">
+    <row r="294" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>292</v>
       </c>
@@ -34194,7 +34206,7 @@
         <v>4301</v>
       </c>
     </row>
-    <row r="295" spans="1:19">
+    <row r="295" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>293</v>
       </c>
@@ -34244,7 +34256,7 @@
         <v>4314</v>
       </c>
     </row>
-    <row r="296" spans="1:19">
+    <row r="296" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>294</v>
       </c>
@@ -34300,7 +34312,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="297" spans="1:19">
+    <row r="297" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>295</v>
       </c>
@@ -34353,7 +34365,7 @@
         <v>4342</v>
       </c>
     </row>
-    <row r="298" spans="1:19">
+    <row r="298" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>296</v>
       </c>
@@ -34409,7 +34421,7 @@
         <v>4357</v>
       </c>
     </row>
-    <row r="299" spans="1:19">
+    <row r="299" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>297</v>
       </c>
@@ -34465,7 +34477,7 @@
         <v>4372</v>
       </c>
     </row>
-    <row r="300" spans="1:19">
+    <row r="300" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>298</v>
       </c>
@@ -34521,7 +34533,7 @@
         <v>4386</v>
       </c>
     </row>
-    <row r="301" spans="1:19">
+    <row r="301" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>299</v>
       </c>
@@ -34577,7 +34589,7 @@
         <v>4401</v>
       </c>
     </row>
-    <row r="302" spans="1:19">
+    <row r="302" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>300</v>
       </c>
@@ -34633,7 +34645,7 @@
         <v>4416</v>
       </c>
     </row>
-    <row r="303" spans="1:19">
+    <row r="303" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>301</v>
       </c>
@@ -34689,7 +34701,7 @@
         <v>4431</v>
       </c>
     </row>
-    <row r="304" spans="1:19">
+    <row r="304" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>302</v>
       </c>
@@ -34742,7 +34754,7 @@
         <v>4445</v>
       </c>
     </row>
-    <row r="305" spans="1:19">
+    <row r="305" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>303</v>
       </c>
@@ -34798,7 +34810,7 @@
         <v>4460</v>
       </c>
     </row>
-    <row r="306" spans="1:19">
+    <row r="306" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>304</v>
       </c>
@@ -34851,7 +34863,7 @@
         <v>4474</v>
       </c>
     </row>
-    <row r="307" spans="1:19">
+    <row r="307" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>305</v>
       </c>
@@ -34907,7 +34919,7 @@
         <v>4488</v>
       </c>
     </row>
-    <row r="308" spans="1:19">
+    <row r="308" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>306</v>
       </c>
@@ -34963,7 +34975,7 @@
         <v>4502</v>
       </c>
     </row>
-    <row r="309" spans="1:19">
+    <row r="309" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>307</v>
       </c>
@@ -35019,7 +35031,7 @@
         <v>4517</v>
       </c>
     </row>
-    <row r="310" spans="1:19">
+    <row r="310" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>308</v>
       </c>
@@ -35075,7 +35087,7 @@
         <v>4532</v>
       </c>
     </row>
-    <row r="311" spans="1:19">
+    <row r="311" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>309</v>
       </c>
@@ -35125,7 +35137,7 @@
         <v>4544</v>
       </c>
     </row>
-    <row r="312" spans="1:19">
+    <row r="312" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>310</v>
       </c>
@@ -35181,7 +35193,7 @@
         <v>4559</v>
       </c>
     </row>
-    <row r="313" spans="1:19">
+    <row r="313" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>311</v>
       </c>
@@ -35237,7 +35249,7 @@
         <v>4574</v>
       </c>
     </row>
-    <row r="314" spans="1:19">
+    <row r="314" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>312</v>
       </c>
@@ -35293,7 +35305,7 @@
         <v>4589</v>
       </c>
     </row>
-    <row r="315" spans="1:19">
+    <row r="315" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>313</v>
       </c>
@@ -35349,7 +35361,7 @@
         <v>4603</v>
       </c>
     </row>
-    <row r="316" spans="1:19">
+    <row r="316" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>314</v>
       </c>
@@ -35405,7 +35417,7 @@
         <v>4618</v>
       </c>
     </row>
-    <row r="317" spans="1:19">
+    <row r="317" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>315</v>
       </c>
@@ -35458,7 +35470,7 @@
         <v>4632</v>
       </c>
     </row>
-    <row r="318" spans="1:19">
+    <row r="318" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>316</v>
       </c>
@@ -35511,7 +35523,7 @@
         <v>4646</v>
       </c>
     </row>
-    <row r="319" spans="1:19">
+    <row r="319" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>317</v>
       </c>
@@ -35567,7 +35579,7 @@
         <v>4661</v>
       </c>
     </row>
-    <row r="320" spans="1:19">
+    <row r="320" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>318</v>
       </c>
@@ -35617,7 +35629,7 @@
         <v>4674</v>
       </c>
     </row>
-    <row r="321" spans="1:19">
+    <row r="321" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>319</v>
       </c>
@@ -35670,7 +35682,7 @@
         <v>4688</v>
       </c>
     </row>
-    <row r="322" spans="1:19">
+    <row r="322" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>320</v>
       </c>
@@ -35723,7 +35735,7 @@
         <v>4702</v>
       </c>
     </row>
-    <row r="323" spans="1:19">
+    <row r="323" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>321</v>
       </c>
@@ -35779,7 +35791,7 @@
         <v>4716</v>
       </c>
     </row>
-    <row r="324" spans="1:19">
+    <row r="324" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>322</v>
       </c>
@@ -35835,7 +35847,7 @@
         <v>4731</v>
       </c>
     </row>
-    <row r="325" spans="1:19">
+    <row r="325" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>323</v>
       </c>
@@ -35891,7 +35903,7 @@
         <v>4746</v>
       </c>
     </row>
-    <row r="326" spans="1:19">
+    <row r="326" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>324</v>
       </c>
@@ -35947,7 +35959,7 @@
         <v>4761</v>
       </c>
     </row>
-    <row r="327" spans="1:19">
+    <row r="327" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>325</v>
       </c>
@@ -36000,7 +36012,7 @@
         <v>4775</v>
       </c>
     </row>
-    <row r="328" spans="1:19">
+    <row r="328" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>326</v>
       </c>
@@ -36056,7 +36068,7 @@
         <v>4790</v>
       </c>
     </row>
-    <row r="329" spans="1:19">
+    <row r="329" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>327</v>
       </c>
@@ -36109,7 +36121,7 @@
         <v>4804</v>
       </c>
     </row>
-    <row r="330" spans="1:19">
+    <row r="330" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>328</v>
       </c>
@@ -36165,7 +36177,7 @@
         <v>4819</v>
       </c>
     </row>
-    <row r="331" spans="1:19">
+    <row r="331" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>329</v>
       </c>
@@ -36221,7 +36233,7 @@
         <v>4834</v>
       </c>
     </row>
-    <row r="332" spans="1:19">
+    <row r="332" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>330</v>
       </c>
@@ -36277,7 +36289,7 @@
         <v>4849</v>
       </c>
     </row>
-    <row r="333" spans="1:19">
+    <row r="333" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>331</v>
       </c>
@@ -36333,7 +36345,7 @@
         <v>4863</v>
       </c>
     </row>
-    <row r="334" spans="1:19">
+    <row r="334" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>332</v>
       </c>
@@ -36386,7 +36398,7 @@
         <v>4876</v>
       </c>
     </row>
-    <row r="335" spans="1:19">
+    <row r="335" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>333</v>
       </c>
@@ -36442,7 +36454,7 @@
         <v>4891</v>
       </c>
     </row>
-    <row r="336" spans="1:19">
+    <row r="336" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>334</v>
       </c>
@@ -36498,7 +36510,7 @@
         <v>4906</v>
       </c>
     </row>
-    <row r="337" spans="1:19">
+    <row r="337" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>335</v>
       </c>
@@ -36554,7 +36566,7 @@
         <v>4921</v>
       </c>
     </row>
-    <row r="338" spans="1:19">
+    <row r="338" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>336</v>
       </c>
@@ -36610,7 +36622,7 @@
         <v>4935</v>
       </c>
     </row>
-    <row r="339" spans="1:19">
+    <row r="339" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>337</v>
       </c>
@@ -36666,7 +36678,7 @@
         <v>4949</v>
       </c>
     </row>
-    <row r="340" spans="1:19">
+    <row r="340" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>338</v>
       </c>
@@ -36716,7 +36728,7 @@
         <v>4961</v>
       </c>
     </row>
-    <row r="341" spans="1:19">
+    <row r="341" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>339</v>
       </c>
@@ -36772,7 +36784,7 @@
         <v>4976</v>
       </c>
     </row>
-    <row r="342" spans="1:19">
+    <row r="342" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>340</v>
       </c>
@@ -36828,7 +36840,7 @@
         <v>4990</v>
       </c>
     </row>
-    <row r="343" spans="1:19">
+    <row r="343" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>341</v>
       </c>
@@ -36884,7 +36896,7 @@
         <v>5005</v>
       </c>
     </row>
-    <row r="344" spans="1:19">
+    <row r="344" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>342</v>
       </c>
@@ -36940,7 +36952,7 @@
         <v>5020</v>
       </c>
     </row>
-    <row r="345" spans="1:19">
+    <row r="345" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>343</v>
       </c>
@@ -36996,7 +37008,7 @@
         <v>5034</v>
       </c>
     </row>
-    <row r="346" spans="1:19">
+    <row r="346" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>344</v>
       </c>
@@ -37046,7 +37058,7 @@
         <v>5046</v>
       </c>
     </row>
-    <row r="347" spans="1:19">
+    <row r="347" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>345</v>
       </c>
@@ -37102,7 +37114,7 @@
         <v>5061</v>
       </c>
     </row>
-    <row r="348" spans="1:19">
+    <row r="348" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>346</v>
       </c>
@@ -37158,7 +37170,7 @@
         <v>5075</v>
       </c>
     </row>
-    <row r="349" spans="1:19">
+    <row r="349" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>347</v>
       </c>
@@ -37214,7 +37226,7 @@
         <v>5090</v>
       </c>
     </row>
-    <row r="350" spans="1:19">
+    <row r="350" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>348</v>
       </c>
@@ -37270,7 +37282,7 @@
         <v>5105</v>
       </c>
     </row>
-    <row r="351" spans="1:19">
+    <row r="351" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>349</v>
       </c>
@@ -37326,7 +37338,7 @@
         <v>5119</v>
       </c>
     </row>
-    <row r="352" spans="1:19">
+    <row r="352" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>350</v>
       </c>
@@ -37382,7 +37394,7 @@
         <v>5134</v>
       </c>
     </row>
-    <row r="353" spans="1:19">
+    <row r="353" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>351</v>
       </c>
@@ -37438,7 +37450,7 @@
         <v>5148</v>
       </c>
     </row>
-    <row r="354" spans="1:19">
+    <row r="354" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>352</v>
       </c>
@@ -37494,7 +37506,7 @@
         <v>5163</v>
       </c>
     </row>
-    <row r="355" spans="1:19">
+    <row r="355" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>353</v>
       </c>
@@ -37550,7 +37562,7 @@
         <v>5178</v>
       </c>
     </row>
-    <row r="356" spans="1:19">
+    <row r="356" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A356">
         <v>354</v>
       </c>
@@ -37603,7 +37615,7 @@
         <v>5191</v>
       </c>
     </row>
-    <row r="357" spans="1:19">
+    <row r="357" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A357">
         <v>355</v>
       </c>
@@ -37653,7 +37665,7 @@
         <v>5203</v>
       </c>
     </row>
-    <row r="358" spans="1:19">
+    <row r="358" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>356</v>
       </c>
@@ -37709,7 +37721,7 @@
         <v>5217</v>
       </c>
     </row>
-    <row r="359" spans="1:19">
+    <row r="359" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A359">
         <v>357</v>
       </c>
@@ -37765,7 +37777,7 @@
         <v>5232</v>
       </c>
     </row>
-    <row r="360" spans="1:19">
+    <row r="360" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A360">
         <v>358</v>
       </c>
@@ -37821,7 +37833,7 @@
         <v>5247</v>
       </c>
     </row>
-    <row r="361" spans="1:19">
+    <row r="361" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A361">
         <v>359</v>
       </c>
@@ -37877,7 +37889,7 @@
         <v>5262</v>
       </c>
     </row>
-    <row r="362" spans="1:19">
+    <row r="362" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A362">
         <v>360</v>
       </c>
@@ -37933,7 +37945,7 @@
         <v>5276</v>
       </c>
     </row>
-    <row r="363" spans="1:19">
+    <row r="363" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A363">
         <v>361</v>
       </c>
@@ -37989,7 +38001,7 @@
         <v>5291</v>
       </c>
     </row>
-    <row r="364" spans="1:19">
+    <row r="364" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>362</v>
       </c>
@@ -38045,7 +38057,7 @@
         <v>5305</v>
       </c>
     </row>
-    <row r="365" spans="1:19">
+    <row r="365" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A365">
         <v>363</v>
       </c>
@@ -38101,7 +38113,7 @@
         <v>5320</v>
       </c>
     </row>
-    <row r="366" spans="1:19">
+    <row r="366" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A366">
         <v>364</v>
       </c>
@@ -38157,7 +38169,7 @@
         <v>5335</v>
       </c>
     </row>
-    <row r="367" spans="1:19">
+    <row r="367" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A367">
         <v>365</v>
       </c>
@@ -38213,7 +38225,7 @@
         <v>5350</v>
       </c>
     </row>
-    <row r="368" spans="1:19">
+    <row r="368" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A368">
         <v>366</v>
       </c>
@@ -38269,7 +38281,7 @@
         <v>5364</v>
       </c>
     </row>
-    <row r="369" spans="1:19">
+    <row r="369" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>367</v>
       </c>
@@ -38322,7 +38334,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="370" spans="1:19">
+    <row r="370" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>368</v>
       </c>
@@ -38378,7 +38390,7 @@
         <v>5391</v>
       </c>
     </row>
-    <row r="371" spans="1:19">
+    <row r="371" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>369</v>
       </c>
@@ -38434,7 +38446,7 @@
         <v>5405</v>
       </c>
     </row>
-    <row r="372" spans="1:19">
+    <row r="372" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A372">
         <v>370</v>
       </c>
@@ -38484,7 +38496,7 @@
         <v>5418</v>
       </c>
     </row>
-    <row r="373" spans="1:19">
+    <row r="373" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>371</v>
       </c>
@@ -38540,7 +38552,7 @@
         <v>5432</v>
       </c>
     </row>
-    <row r="374" spans="1:19">
+    <row r="374" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A374">
         <v>372</v>
       </c>
@@ -38596,7 +38608,7 @@
         <v>5447</v>
       </c>
     </row>
-    <row r="375" spans="1:19">
+    <row r="375" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A375">
         <v>373</v>
       </c>
@@ -38652,7 +38664,7 @@
         <v>5461</v>
       </c>
     </row>
-    <row r="376" spans="1:19">
+    <row r="376" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>374</v>
       </c>
@@ -38708,7 +38720,7 @@
         <v>5475</v>
       </c>
     </row>
-    <row r="377" spans="1:19">
+    <row r="377" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>375</v>
       </c>
@@ -38761,7 +38773,7 @@
         <v>5488</v>
       </c>
     </row>
-    <row r="378" spans="1:19">
+    <row r="378" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>376</v>
       </c>
@@ -38817,7 +38829,7 @@
         <v>5501</v>
       </c>
     </row>
-    <row r="379" spans="1:19">
+    <row r="379" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>377</v>
       </c>
@@ -38873,7 +38885,7 @@
         <v>5516</v>
       </c>
     </row>
-    <row r="380" spans="1:19">
+    <row r="380" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>378</v>
       </c>
@@ -38926,7 +38938,7 @@
         <v>5529</v>
       </c>
     </row>
-    <row r="381" spans="1:19">
+    <row r="381" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>379</v>
       </c>
@@ -38982,7 +38994,7 @@
         <v>5543</v>
       </c>
     </row>
-    <row r="382" spans="1:19">
+    <row r="382" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>380</v>
       </c>
@@ -39038,7 +39050,7 @@
         <v>5558</v>
       </c>
     </row>
-    <row r="383" spans="1:19">
+    <row r="383" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>381</v>
       </c>
@@ -39094,7 +39106,7 @@
         <v>5573</v>
       </c>
     </row>
-    <row r="384" spans="1:19">
+    <row r="384" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>382</v>
       </c>
@@ -39150,7 +39162,7 @@
         <v>5588</v>
       </c>
     </row>
-    <row r="385" spans="1:19">
+    <row r="385" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>383</v>
       </c>
@@ -39206,7 +39218,7 @@
         <v>5603</v>
       </c>
     </row>
-    <row r="386" spans="1:19">
+    <row r="386" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A386">
         <v>384</v>
       </c>
@@ -39262,7 +39274,7 @@
         <v>5618</v>
       </c>
     </row>
-    <row r="387" spans="1:19">
+    <row r="387" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A387">
         <v>385</v>
       </c>
@@ -39318,7 +39330,7 @@
         <v>5633</v>
       </c>
     </row>
-    <row r="388" spans="1:19">
+    <row r="388" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A388">
         <v>386</v>
       </c>
@@ -39374,7 +39386,7 @@
         <v>5648</v>
       </c>
     </row>
-    <row r="389" spans="1:19">
+    <row r="389" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A389">
         <v>387</v>
       </c>
@@ -39430,7 +39442,7 @@
         <v>5663</v>
       </c>
     </row>
-    <row r="390" spans="1:19">
+    <row r="390" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A390">
         <v>388</v>
       </c>
@@ -39486,7 +39498,7 @@
         <v>5678</v>
       </c>
     </row>
-    <row r="391" spans="1:19">
+    <row r="391" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A391">
         <v>389</v>
       </c>
@@ -39542,7 +39554,7 @@
         <v>5693</v>
       </c>
     </row>
-    <row r="392" spans="1:19">
+    <row r="392" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A392">
         <v>390</v>
       </c>
@@ -39595,7 +39607,7 @@
         <v>5707</v>
       </c>
     </row>
-    <row r="393" spans="1:19">
+    <row r="393" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A393">
         <v>391</v>
       </c>
@@ -39651,7 +39663,7 @@
         <v>5722</v>
       </c>
     </row>
-    <row r="394" spans="1:19">
+    <row r="394" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A394">
         <v>392</v>
       </c>
@@ -39704,7 +39716,7 @@
         <v>5736</v>
       </c>
     </row>
-    <row r="395" spans="1:19">
+    <row r="395" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A395">
         <v>393</v>
       </c>
@@ -39757,7 +39769,7 @@
         <v>5750</v>
       </c>
     </row>
-    <row r="396" spans="1:19">
+    <row r="396" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A396">
         <v>394</v>
       </c>
@@ -39813,7 +39825,7 @@
         <v>5764</v>
       </c>
     </row>
-    <row r="397" spans="1:19">
+    <row r="397" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A397">
         <v>395</v>
       </c>
@@ -39869,7 +39881,7 @@
         <v>5778</v>
       </c>
     </row>
-    <row r="398" spans="1:19">
+    <row r="398" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A398">
         <v>396</v>
       </c>
@@ -39925,7 +39937,7 @@
         <v>5793</v>
       </c>
     </row>
-    <row r="399" spans="1:19">
+    <row r="399" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A399">
         <v>397</v>
       </c>
@@ -39981,7 +39993,7 @@
         <v>5808</v>
       </c>
     </row>
-    <row r="400" spans="1:19">
+    <row r="400" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A400">
         <v>398</v>
       </c>
@@ -40037,7 +40049,7 @@
         <v>5821</v>
       </c>
     </row>
-    <row r="401" spans="1:19">
+    <row r="401" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A401">
         <v>399</v>
       </c>
@@ -40089,10 +40101,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>